<commit_message>
~ update BOM caravel REV5B
</commit_message>
<xml_diff>
--- a/hardware/development/caravel-dev-v5-M.2/caravel-dev-v5-M.2.xlsx
+++ b/hardware/development/caravel-dev-v5-M.2/caravel-dev-v5-M.2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t xml:space="preserve">Manufacturer Part Number</t>
   </si>
@@ -232,13 +232,19 @@
     <t xml:space="preserve">HDR100IMP40M-G-V-TH</t>
   </si>
   <si>
-    <t xml:space="preserve">J10</t>
+    <t xml:space="preserve">J10, J11</t>
   </si>
   <si>
     <t xml:space="preserve">Loose Part</t>
   </si>
   <si>
-    <t xml:space="preserve">J11</t>
+    <t xml:space="preserve">Standoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screw</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -316,6 +322,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
@@ -391,7 +404,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -436,7 +449,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,16 +461,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -471,30 +496,6 @@
     <cellStyle name="Hyperlink 2" xfId="21"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7F7F7"/>
-          <bgColor rgb="FF272727"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9F9F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -563,10 +564,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,10 +576,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="9.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="9.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -620,9 +623,10 @@
       <c r="C2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="11"/>
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
@@ -630,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <v>2</v>
       </c>
@@ -640,13 +644,13 @@
       <c r="C3" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="11"/>
       <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
@@ -664,9 +668,10 @@
       <c r="C4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="E4" s="11"/>
       <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
@@ -684,9 +689,10 @@
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="11"/>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
@@ -707,9 +713,10 @@
       <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="E6" s="11"/>
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
@@ -727,29 +734,34 @@
       <c r="C7" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="E7" s="11"/>
       <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
+      <c r="E8" s="11"/>
       <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
@@ -761,16 +773,16 @@
       <c r="A9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -784,16 +796,16 @@
       <c r="A10" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="11" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -807,16 +819,16 @@
       <c r="A11" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -830,16 +842,16 @@
       <c r="A12" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -854,16 +866,16 @@
       <c r="A13" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="11" t="s">
         <v>43</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -877,16 +889,16 @@
       <c r="A14" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="11" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -900,16 +912,16 @@
       <c r="A15" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="12" t="n">
+      <c r="E15" s="13" t="n">
         <v>150</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -923,16 +935,16 @@
       <c r="A16" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -946,16 +958,16 @@
       <c r="A17" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -964,7 +976,7 @@
       <c r="H17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="0"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="n">
@@ -976,9 +988,10 @@
       <c r="C18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="E18" s="11"/>
       <c r="F18" s="3" t="s">
         <v>11</v>
       </c>
@@ -996,17 +1009,17 @@
       <c r="C19" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13" t="s">
+      <c r="G19" s="11"/>
+      <c r="H19" s="11" t="s">
         <v>60</v>
       </c>
       <c r="I19" s="9"/>
@@ -1021,10 +1034,10 @@
       <c r="C20" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="11" t="s">
         <v>63</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1044,9 +1057,10 @@
       <c r="C21" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="E21" s="11"/>
       <c r="F21" s="3" t="s">
         <v>11</v>
       </c>
@@ -1064,9 +1078,10 @@
       <c r="C22" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="E22" s="11"/>
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1083,11 +1098,12 @@
         <v>68</v>
       </c>
       <c r="C23" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>69</v>
       </c>
+      <c r="E23" s="11"/>
       <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
@@ -1099,30 +1115,38 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="n">
+      <c r="A24" s="16" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="B24" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>70</v>
+      <c r="C24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="I25" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
@@ -1130,47 +1154,49 @@
     </row>
     <row r="27" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="9"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="10"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="10"/>
-      <c r="D31" s="16"/>
+      <c r="D31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="10"/>
-      <c r="D32" s="16"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="10"/>
-      <c r="D33" s="16"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="10"/>
-      <c r="D34" s="16"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="10"/>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10"/>
-      <c r="D36" s="9"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="FT232HQ"/>
     <hyperlink ref="B3" r:id="rId2" display="SN74LVC1G125DCKT"/>
@@ -1178,23 +1204,27 @@
     <hyperlink ref="B5" r:id="rId4" display="TAR5S18U"/>
     <hyperlink ref="B6" r:id="rId5" display="W25Q32JVSSIQ"/>
     <hyperlink ref="B7" r:id="rId6" display="M.2 E connector"/>
-    <hyperlink ref="B8" r:id="rId7" display="APT3216SURCK"/>
-    <hyperlink ref="B9" r:id="rId8" display="CL21B106KAYQNNE"/>
-    <hyperlink ref="B10" r:id="rId9" display="885012207103"/>
-    <hyperlink ref="B11" r:id="rId10" display="C0805C104K5RAC7411"/>
-    <hyperlink ref="B12" r:id="rId11" display="C0805C103K5RAC7411"/>
-    <hyperlink ref="B13" r:id="rId12" display="RC0805FR-0710KL"/>
-    <hyperlink ref="B14" r:id="rId13" display="RMCF0805FT12K0"/>
-    <hyperlink ref="B15" r:id="rId14" display="RNCP0805FTD150R"/>
-    <hyperlink ref="B16" r:id="rId15" display="RC0805FR-071KL"/>
-    <hyperlink ref="B17" r:id="rId16" display="7427920415"/>
-    <hyperlink ref="B18" r:id="rId17" display="10118193-0001LF"/>
-    <hyperlink ref="B19" r:id="rId18" display="DSC6001JI1B-010.0000"/>
-    <hyperlink ref="B20" r:id="rId19" display="CSTNE12M0GH5L000R0"/>
-    <hyperlink ref="B21" r:id="rId20" display="36-5000-ND"/>
-    <hyperlink ref="B22" r:id="rId21" display="SKQGADE010"/>
-    <hyperlink ref="B23" r:id="rId22" display="HDR100IMP40M-G-V-TH"/>
-    <hyperlink ref="B24" r:id="rId23" display="HDR100IMP40M-G-V-TH"/>
+    <hyperlink ref="I7" r:id="rId7" display="alternative part"/>
+    <hyperlink ref="B8" r:id="rId8" display="APT3216SURCK"/>
+    <hyperlink ref="B9" r:id="rId9" display="CL21B106KAYQNNE"/>
+    <hyperlink ref="B10" r:id="rId10" display="885012207103"/>
+    <hyperlink ref="B11" r:id="rId11" display="C0805C104K5RAC7411"/>
+    <hyperlink ref="B12" r:id="rId12" display="C0805C103K5RAC7411"/>
+    <hyperlink ref="B13" r:id="rId13" display="RC0805FR-0710KL"/>
+    <hyperlink ref="B14" r:id="rId14" display="RMCF0805FT12K0"/>
+    <hyperlink ref="B15" r:id="rId15" display="RNCP0805FTD150R"/>
+    <hyperlink ref="B16" r:id="rId16" display="RC0805FR-071KL"/>
+    <hyperlink ref="B17" r:id="rId17" display="7427920415"/>
+    <hyperlink ref="B18" r:id="rId18" display="10118193-0001LF"/>
+    <hyperlink ref="B19" r:id="rId19" display="DSC6001JI1B-010.0000"/>
+    <hyperlink ref="B20" r:id="rId20" display="CSTNE12M0GH5L000R0"/>
+    <hyperlink ref="B21" r:id="rId21" display="36-5000-ND"/>
+    <hyperlink ref="B22" r:id="rId22" display="SKQGADE010"/>
+    <hyperlink ref="B23" r:id="rId23" display="HDR100IMP40M-G-V-TH"/>
+    <hyperlink ref="B24" r:id="rId24" display="Standoff"/>
+    <hyperlink ref="I24" r:id="rId25" display="alternative part"/>
+    <hyperlink ref="B25" r:id="rId26" display="Screw"/>
+    <hyperlink ref="I25" r:id="rId27" display="alternative part"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>